<commit_message>
Worked on reroute request functionality
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageOrdersTestData.xlsx
+++ b/binaries/FCfiles/ManageOrdersTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14430" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13170" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Reroute Request" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Location Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>#123, Los Angeles</t>
   </si>
   <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
     <t>AL</t>
   </si>
   <si>
@@ -71,6 +68,66 @@
   </si>
   <si>
     <t>Amazon FBA Warehouse</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Way Bill #</t>
+  </si>
+  <si>
+    <t>CEV1002186</t>
+  </si>
+  <si>
+    <t>90001</t>
+  </si>
+  <si>
+    <t>Test Location 2</t>
+  </si>
+  <si>
+    <t>#123, Moody</t>
+  </si>
+  <si>
+    <t>Test Location 3</t>
+  </si>
+  <si>
+    <t>#321, Los Angeles</t>
+  </si>
+  <si>
+    <t>Earliest Drop-Off</t>
+  </si>
+  <si>
+    <t>Latest Drop-Off</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>51487615</t>
+  </si>
+  <si>
+    <t>51488422</t>
+  </si>
+  <si>
+    <t>51488421</t>
+  </si>
+  <si>
+    <t>66488699</t>
+  </si>
+  <si>
+    <t>66488700</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>orderReferenceID</t>
+  </si>
+  <si>
+    <t>LOS ANGELES</t>
+  </si>
+  <si>
+    <t>MOODY</t>
   </si>
 </sst>
 </file>
@@ -106,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,85 +461,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
+      <c r="J3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Completed BOL cancellation ticket
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageOrdersTestData.xlsx
+++ b/binaries/FCfiles/ManageOrdersTestData.xlsx
@@ -2,22 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13170" windowHeight="6330"/>
+    <workbookView activeTab="1" windowHeight="6330" windowWidth="15480" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="Reroute Request" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Reroute Request" r:id="rId1" sheetId="1"/>
+    <sheet name="BOL" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Location Name</t>
   </si>
@@ -128,12 +127,52 @@
   </si>
   <si>
     <t>MOODY</t>
+  </si>
+  <si>
+    <t>LTL Order</t>
+  </si>
+  <si>
+    <t>Parcel</t>
+  </si>
+  <si>
+    <t>Shipment Type</t>
+  </si>
+  <si>
+    <t>Starting tracking number</t>
+  </si>
+  <si>
+    <t>1z</t>
+  </si>
+  <si>
+    <t>Order Status</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>51488766</t>
+  </si>
+  <si>
+    <t>51488767</t>
+  </si>
+  <si>
+    <t>51488769</t>
+  </si>
+  <si>
+    <t>fces</t>
+  </si>
+  <si>
+    <t>51488755</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -143,15 +182,25 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,20 +208,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="11">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -181,10 +256,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -340,7 +415,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -349,13 +424,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -365,7 +440,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -374,7 +449,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -383,7 +458,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -393,12 +468,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -429,7 +504,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -448,7 +523,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -461,27 +536,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -634,20 +709,81 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -659,6 +795,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scroll added in log off
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageOrdersTestData.xlsx
+++ b/binaries/FCfiles/ManageOrdersTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Location Name</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>51492405</t>
+  </si>
+  <si>
+    <t>51499682</t>
+  </si>
+  <si>
+    <t>51492012</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
@@ -241,6 +247,9 @@
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -752,8 +761,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
-        <v>44</v>
+      <c r="A2" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -763,8 +772,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="12" t="s">
-        <v>45</v>
+      <c r="A3" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -777,8 +786,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
-        <v>45</v>
+      <c r="A4" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Merging of Manage Billing Tests and some script updates
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageOrdersTestData.xlsx
+++ b/binaries/FCfiles/ManageOrdersTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Location Name</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>51487044</t>
+  </si>
+  <si>
+    <t>51521969</t>
+  </si>
+  <si>
+    <t>51486557</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
@@ -283,6 +289,9 @@
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -815,8 +824,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="31" t="s">
-        <v>58</v>
+      <c r="A2" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -826,8 +835,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="33" t="s">
-        <v>59</v>
+      <c r="A3" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -840,8 +849,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="32" t="s">
-        <v>59</v>
+      <c r="A4" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>

</xml_diff>